<commit_message>
Diagrma de secuencias, uml arreglados, progreso programacion
</commit_message>
<xml_diff>
--- a/tlog.xlsx
+++ b/tlog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Fecha</t>
   </si>
@@ -51,6 +51,14 @@
   <si>
     <t>Clases Sort
 main</t>
+  </si>
+  <si>
+    <t>modificacion
+UML</t>
+  </si>
+  <si>
+    <t>diagrama de
+secuencias</t>
   </si>
 </sst>
 </file>
@@ -407,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -478,6 +486,66 @@
         <v>8</v>
       </c>
     </row>
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>42580</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.11458333333333333</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.11666666666666665</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>42580</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.11805555555555557</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>68</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>42580</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.17708333333333334</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.3125</v>
+      </c>
+      <c r="D6">
+        <v>30</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.11458333333333333</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>